<commit_message>
change website name in import test
</commit_message>
<xml_diff>
--- a/changedetectionio/tests/import/spreadsheet.xlsx
+++ b/changedetectionio/tests/import/spreadsheet.xlsx
@@ -88,7 +88,7 @@
     <t xml:space="preserve">https://www.cooeeelnews.com/?pid=foobarxxx</t>
   </si>
   <si>
-    <t xml:space="preserve">Dyn Test</t>
+    <t xml:space="preserve">system default website</t>
   </si>
   <si>
     <t xml:space="preserve">00133f47-76a9-4ab2-84a7-a68abc176b72</t>
@@ -106,7 +106,7 @@
     <numFmt numFmtId="165" formatCode="General"/>
     <numFmt numFmtId="166" formatCode="d/mm/yyyy\ h:mm"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -152,13 +152,6 @@
       <family val="0"/>
       <charset val="1"/>
     </font>
-    <font>
-      <u val="single"/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Cambria"/>
-      <family val="0"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -202,7 +195,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -227,10 +220,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -251,7 +240,7 @@
   <dimension ref="A1:J1000"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G5" activeCellId="0" sqref="G5:J5"/>
+      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.37890625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -401,7 +390,7 @@
       <c r="A5" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="3" t="s">
         <v>23</v>
       </c>
       <c r="C5" s="2" t="s">

</xml_diff>